<commit_message>
add multiple string to excel
</commit_message>
<xml_diff>
--- a/Tax/data/test.xlsx
+++ b/Tax/data/test.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,6 +433,105 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Всё</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>хорошо</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>прекрасная</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>маркиза!</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Все</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>хорошо,</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>все</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>хорошо</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Readings</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>to</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>make</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>your</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Life</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>best</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>can</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>be</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>